<commit_message>
Modified input data to show interaction of growth and shift rates
</commit_message>
<xml_diff>
--- a/output/test_output_file.xlsx
+++ b/output/test_output_file.xlsx
@@ -6187,19 +6187,19 @@
         <v>1</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>39208</v>
+        <v>40000</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>792</v>
+        <v>0</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>105.34</v>
+        <v>0</v>
       </c>
       <c r="G3" s="2" t="n">
-        <v>0.07</v>
+        <v>0</v>
       </c>
       <c r="H3" s="2" t="n">
-        <v>0.07</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -6213,19 +6213,19 @@
         <v>2</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>38432</v>
+        <v>40000</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>776</v>
+        <v>0</v>
       </c>
       <c r="F4" s="2" t="n">
-        <v>103.21</v>
+        <v>0</v>
       </c>
       <c r="G4" s="2" t="n">
-        <v>0.07</v>
+        <v>0</v>
       </c>
       <c r="H4" s="2" t="n">
-        <v>0.14</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -6239,19 +6239,19 @@
         <v>3</v>
       </c>
       <c r="D5" s="2" t="n">
-        <v>37671</v>
+        <v>40000</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>761</v>
+        <v>0</v>
       </c>
       <c r="F5" s="2" t="n">
-        <v>101.21</v>
+        <v>0</v>
       </c>
       <c r="G5" s="2" t="n">
-        <v>0.07</v>
+        <v>0</v>
       </c>
       <c r="H5" s="2" t="n">
-        <v>0.21</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -6265,19 +6265,19 @@
         <v>4</v>
       </c>
       <c r="D6" s="2" t="n">
-        <v>36925</v>
+        <v>40000</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>746</v>
+        <v>0</v>
       </c>
       <c r="F6" s="2" t="n">
-        <v>99.22</v>
+        <v>0</v>
       </c>
       <c r="G6" s="2" t="n">
-        <v>0.07</v>
+        <v>0</v>
       </c>
       <c r="H6" s="2" t="n">
-        <v>0.28</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -6291,19 +6291,19 @@
         <v>5</v>
       </c>
       <c r="D7" s="2" t="n">
-        <v>36194</v>
+        <v>40000</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>731</v>
+        <v>0</v>
       </c>
       <c r="F7" s="2" t="n">
-        <v>97.22</v>
+        <v>0</v>
       </c>
       <c r="G7" s="2" t="n">
-        <v>0.07</v>
+        <v>0</v>
       </c>
       <c r="H7" s="2" t="n">
-        <v>0.35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -6317,19 +6317,19 @@
         <v>6</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>35477</v>
+        <v>40000</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>717</v>
+        <v>0</v>
       </c>
       <c r="F8" s="2" t="n">
-        <v>95.36</v>
+        <v>0</v>
       </c>
       <c r="G8" s="2" t="n">
-        <v>0.07</v>
+        <v>0</v>
       </c>
       <c r="H8" s="2" t="n">
-        <v>0.42</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -6343,19 +6343,19 @@
         <v>7</v>
       </c>
       <c r="D9" s="2" t="n">
-        <v>34775</v>
+        <v>40000</v>
       </c>
       <c r="E9" s="2" t="n">
-        <v>702</v>
+        <v>0</v>
       </c>
       <c r="F9" s="2" t="n">
-        <v>93.37</v>
+        <v>0</v>
       </c>
       <c r="G9" s="2" t="n">
-        <v>0.06</v>
+        <v>0</v>
       </c>
       <c r="H9" s="2" t="n">
-        <v>0.48</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -6369,19 +6369,19 @@
         <v>8</v>
       </c>
       <c r="D10" s="2" t="n">
-        <v>34086</v>
+        <v>40000</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>689</v>
+        <v>0</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>91.64</v>
+        <v>0</v>
       </c>
       <c r="G10" s="2" t="n">
-        <v>0.06</v>
+        <v>0</v>
       </c>
       <c r="H10" s="2" t="n">
-        <v>0.54</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -6395,19 +6395,19 @@
         <v>9</v>
       </c>
       <c r="D11" s="2" t="n">
-        <v>33411</v>
+        <v>40000</v>
       </c>
       <c r="E11" s="2" t="n">
-        <v>675</v>
+        <v>0</v>
       </c>
       <c r="F11" s="2" t="n">
-        <v>89.78</v>
+        <v>0</v>
       </c>
       <c r="G11" s="2" t="n">
-        <v>0.06</v>
+        <v>0</v>
       </c>
       <c r="H11" s="2" t="n">
-        <v>0.6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -6421,19 +6421,19 @@
         <v>10</v>
       </c>
       <c r="D12" s="2" t="n">
-        <v>32750</v>
+        <v>40000</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>661</v>
+        <v>0</v>
       </c>
       <c r="F12" s="2" t="n">
-        <v>87.91</v>
+        <v>0</v>
       </c>
       <c r="G12" s="2" t="n">
-        <v>0.06</v>
+        <v>0</v>
       </c>
       <c r="H12" s="2" t="n">
-        <v>0.66</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -6447,19 +6447,19 @@
         <v>11</v>
       </c>
       <c r="D13" s="2" t="n">
-        <v>32101</v>
+        <v>40000</v>
       </c>
       <c r="E13" s="2" t="n">
-        <v>649</v>
+        <v>0</v>
       </c>
       <c r="F13" s="2" t="n">
-        <v>86.32</v>
+        <v>0</v>
       </c>
       <c r="G13" s="2" t="n">
-        <v>0.06</v>
+        <v>0</v>
       </c>
       <c r="H13" s="2" t="n">
-        <v>0.72</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -6473,19 +6473,19 @@
         <v>12</v>
       </c>
       <c r="D14" s="2" t="n">
-        <v>31466</v>
+        <v>40000</v>
       </c>
       <c r="E14" s="2" t="n">
-        <v>635</v>
+        <v>0</v>
       </c>
       <c r="F14" s="2" t="n">
-        <v>84.46</v>
+        <v>0</v>
       </c>
       <c r="G14" s="2" t="n">
-        <v>0.06</v>
+        <v>0</v>
       </c>
       <c r="H14" s="2" t="n">
-        <v>0.78</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -6499,19 +6499,19 @@
         <v>13</v>
       </c>
       <c r="D15" s="2" t="n">
-        <v>30843</v>
+        <v>40000</v>
       </c>
       <c r="E15" s="2" t="n">
-        <v>623</v>
+        <v>0</v>
       </c>
       <c r="F15" s="2" t="n">
-        <v>82.86</v>
+        <v>0</v>
       </c>
       <c r="G15" s="2" t="n">
-        <v>0.06</v>
+        <v>0</v>
       </c>
       <c r="H15" s="2" t="n">
-        <v>0.84</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -6525,19 +6525,19 @@
         <v>14</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>30232</v>
+        <v>40000</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>611</v>
+        <v>0</v>
       </c>
       <c r="F16" s="2" t="n">
-        <v>81.26</v>
+        <v>0</v>
       </c>
       <c r="G16" s="2" t="n">
-        <v>0.06</v>
+        <v>0</v>
       </c>
       <c r="H16" s="2" t="n">
-        <v>0.9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -6551,19 +6551,19 @@
         <v>15</v>
       </c>
       <c r="D17" s="2" t="n">
-        <v>29634</v>
+        <v>40000</v>
       </c>
       <c r="E17" s="2" t="n">
-        <v>598</v>
+        <v>0</v>
       </c>
       <c r="F17" s="2" t="n">
-        <v>79.53</v>
+        <v>0</v>
       </c>
       <c r="G17" s="2" t="n">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="H17" s="2" t="n">
-        <v>0.95</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -6577,19 +6577,19 @@
         <v>16</v>
       </c>
       <c r="D18" s="2" t="n">
-        <v>29047</v>
+        <v>40000</v>
       </c>
       <c r="E18" s="2" t="n">
-        <v>587</v>
+        <v>0</v>
       </c>
       <c r="F18" s="2" t="n">
-        <v>78.07</v>
+        <v>0</v>
       </c>
       <c r="G18" s="2" t="n">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="H18" s="2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -6603,19 +6603,19 @@
         <v>17</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>28472</v>
+        <v>40000</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>575</v>
+        <v>0</v>
       </c>
       <c r="F19" s="2" t="n">
-        <v>76.48</v>
+        <v>0</v>
       </c>
       <c r="G19" s="2" t="n">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="H19" s="2" t="n">
-        <v>1.05</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -6629,19 +6629,19 @@
         <v>18</v>
       </c>
       <c r="D20" s="2" t="n">
-        <v>27908</v>
+        <v>40000</v>
       </c>
       <c r="E20" s="2" t="n">
-        <v>564</v>
+        <v>0</v>
       </c>
       <c r="F20" s="2" t="n">
-        <v>75.01</v>
+        <v>0</v>
       </c>
       <c r="G20" s="2" t="n">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="H20" s="2" t="n">
-        <v>1.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -6655,19 +6655,19 @@
         <v>19</v>
       </c>
       <c r="D21" s="2" t="n">
-        <v>27356</v>
+        <v>40000</v>
       </c>
       <c r="E21" s="2" t="n">
-        <v>552</v>
+        <v>0</v>
       </c>
       <c r="F21" s="2" t="n">
-        <v>73.42</v>
+        <v>0</v>
       </c>
       <c r="G21" s="2" t="n">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="H21" s="2" t="n">
-        <v>1.15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
@@ -6681,19 +6681,19 @@
         <v>20</v>
       </c>
       <c r="D22" s="2" t="n">
-        <v>26814</v>
+        <v>40000</v>
       </c>
       <c r="E22" s="2" t="n">
-        <v>542</v>
+        <v>0</v>
       </c>
       <c r="F22" s="2" t="n">
-        <v>72.09</v>
+        <v>0</v>
       </c>
       <c r="G22" s="2" t="n">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="H22" s="2" t="n">
-        <v>1.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23">
@@ -6707,19 +6707,19 @@
         <v>21</v>
       </c>
       <c r="D23" s="2" t="n">
-        <v>26283</v>
+        <v>40000</v>
       </c>
       <c r="E23" s="2" t="n">
-        <v>531</v>
+        <v>0</v>
       </c>
       <c r="F23" s="2" t="n">
-        <v>70.62</v>
+        <v>0</v>
       </c>
       <c r="G23" s="2" t="n">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="H23" s="2" t="n">
-        <v>1.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
@@ -6733,19 +6733,19 @@
         <v>22</v>
       </c>
       <c r="D24" s="2" t="n">
-        <v>25763</v>
+        <v>40000</v>
       </c>
       <c r="E24" s="2" t="n">
-        <v>520</v>
+        <v>0</v>
       </c>
       <c r="F24" s="2" t="n">
-        <v>69.16</v>
+        <v>0</v>
       </c>
       <c r="G24" s="2" t="n">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="H24" s="2" t="n">
-        <v>1.3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -6759,19 +6759,19 @@
         <v>23</v>
       </c>
       <c r="D25" s="2" t="n">
-        <v>25253</v>
+        <v>40000</v>
       </c>
       <c r="E25" s="2" t="n">
-        <v>510</v>
+        <v>0</v>
       </c>
       <c r="F25" s="2" t="n">
-        <v>67.83</v>
+        <v>0</v>
       </c>
       <c r="G25" s="2" t="n">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="H25" s="2" t="n">
-        <v>1.35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26">
@@ -6785,19 +6785,19 @@
         <v>24</v>
       </c>
       <c r="D26" s="2" t="n">
-        <v>24753</v>
+        <v>40000</v>
       </c>
       <c r="E26" s="2" t="n">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="F26" s="2" t="n">
-        <v>66.5</v>
+        <v>0</v>
       </c>
       <c r="G26" s="2" t="n">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="H26" s="2" t="n">
-        <v>1.4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27">
@@ -6811,19 +6811,19 @@
         <v>25</v>
       </c>
       <c r="D27" s="2" t="n">
-        <v>24262</v>
+        <v>40000</v>
       </c>
       <c r="E27" s="2" t="n">
-        <v>491</v>
+        <v>0</v>
       </c>
       <c r="F27" s="2" t="n">
-        <v>65.3</v>
+        <v>0</v>
       </c>
       <c r="G27" s="2" t="n">
-        <v>0.04</v>
+        <v>0</v>
       </c>
       <c r="H27" s="2" t="n">
-        <v>1.44</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28">
@@ -6837,19 +6837,19 @@
         <v>26</v>
       </c>
       <c r="D28" s="2" t="n">
-        <v>23782</v>
+        <v>40000</v>
       </c>
       <c r="E28" s="2" t="n">
-        <v>480</v>
+        <v>0</v>
       </c>
       <c r="F28" s="2" t="n">
-        <v>63.84</v>
+        <v>0</v>
       </c>
       <c r="G28" s="2" t="n">
-        <v>0.04</v>
+        <v>0</v>
       </c>
       <c r="H28" s="2" t="n">
-        <v>1.48</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29">
@@ -6863,19 +6863,19 @@
         <v>27</v>
       </c>
       <c r="D29" s="2" t="n">
-        <v>23311</v>
+        <v>40000</v>
       </c>
       <c r="E29" s="2" t="n">
-        <v>471</v>
+        <v>0</v>
       </c>
       <c r="F29" s="2" t="n">
-        <v>62.64</v>
+        <v>0</v>
       </c>
       <c r="G29" s="2" t="n">
-        <v>0.04</v>
+        <v>0</v>
       </c>
       <c r="H29" s="2" t="n">
-        <v>1.52</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30">
@@ -6889,19 +6889,19 @@
         <v>28</v>
       </c>
       <c r="D30" s="2" t="n">
-        <v>22850</v>
+        <v>40000</v>
       </c>
       <c r="E30" s="2" t="n">
-        <v>461</v>
+        <v>0</v>
       </c>
       <c r="F30" s="2" t="n">
-        <v>61.31</v>
+        <v>0</v>
       </c>
       <c r="G30" s="2" t="n">
-        <v>0.04</v>
+        <v>0</v>
       </c>
       <c r="H30" s="2" t="n">
-        <v>1.56</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31">
@@ -6915,19 +6915,19 @@
         <v>29</v>
       </c>
       <c r="D31" s="2" t="n">
-        <v>22397</v>
+        <v>40000</v>
       </c>
       <c r="E31" s="2" t="n">
-        <v>453</v>
+        <v>0</v>
       </c>
       <c r="F31" s="2" t="n">
-        <v>60.25</v>
+        <v>0</v>
       </c>
       <c r="G31" s="2" t="n">
-        <v>0.04</v>
+        <v>0</v>
       </c>
       <c r="H31" s="2" t="n">
-        <v>1.6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32">
@@ -6941,19 +6941,19 @@
         <v>30</v>
       </c>
       <c r="D32" s="2" t="n">
-        <v>21954</v>
+        <v>40000</v>
       </c>
       <c r="E32" s="2" t="n">
-        <v>443</v>
+        <v>0</v>
       </c>
       <c r="F32" s="2" t="n">
-        <v>58.92</v>
+        <v>0</v>
       </c>
       <c r="G32" s="2" t="n">
-        <v>0.04</v>
+        <v>0</v>
       </c>
       <c r="H32" s="2" t="n">
-        <v>1.64</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33">
@@ -6967,19 +6967,19 @@
         <v>31</v>
       </c>
       <c r="D33" s="2" t="n">
-        <v>21519</v>
+        <v>40000</v>
       </c>
       <c r="E33" s="2" t="n">
-        <v>435</v>
+        <v>0</v>
       </c>
       <c r="F33" s="2" t="n">
-        <v>57.86</v>
+        <v>0</v>
       </c>
       <c r="G33" s="2" t="n">
-        <v>0.04</v>
+        <v>0</v>
       </c>
       <c r="H33" s="2" t="n">
-        <v>1.68</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34">
@@ -6993,19 +6993,19 @@
         <v>32</v>
       </c>
       <c r="D34" s="2" t="n">
-        <v>21093</v>
+        <v>40000</v>
       </c>
       <c r="E34" s="2" t="n">
-        <v>426</v>
+        <v>0</v>
       </c>
       <c r="F34" s="2" t="n">
-        <v>56.66</v>
+        <v>0</v>
       </c>
       <c r="G34" s="2" t="n">
-        <v>0.04</v>
+        <v>0</v>
       </c>
       <c r="H34" s="2" t="n">
-        <v>1.72</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35">
@@ -7019,19 +7019,19 @@
         <v>33</v>
       </c>
       <c r="D35" s="2" t="n">
-        <v>20675</v>
+        <v>40000</v>
       </c>
       <c r="E35" s="2" t="n">
-        <v>418</v>
+        <v>0</v>
       </c>
       <c r="F35" s="2" t="n">
-        <v>55.59</v>
+        <v>0</v>
       </c>
       <c r="G35" s="2" t="n">
-        <v>0.04</v>
+        <v>0</v>
       </c>
       <c r="H35" s="2" t="n">
-        <v>1.76</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36">
@@ -7045,19 +7045,19 @@
         <v>34</v>
       </c>
       <c r="D36" s="2" t="n">
-        <v>20266</v>
+        <v>40000</v>
       </c>
       <c r="E36" s="2" t="n">
-        <v>409</v>
+        <v>0</v>
       </c>
       <c r="F36" s="2" t="n">
-        <v>54.4</v>
+        <v>0</v>
       </c>
       <c r="G36" s="2" t="n">
-        <v>0.04</v>
+        <v>0</v>
       </c>
       <c r="H36" s="2" t="n">
-        <v>1.8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37">
@@ -7071,19 +7071,19 @@
         <v>35</v>
       </c>
       <c r="D37" s="2" t="n">
-        <v>19865</v>
+        <v>40000</v>
       </c>
       <c r="E37" s="2" t="n">
-        <v>401</v>
+        <v>0</v>
       </c>
       <c r="F37" s="2" t="n">
-        <v>53.33</v>
+        <v>0</v>
       </c>
       <c r="G37" s="2" t="n">
-        <v>0.04</v>
+        <v>0</v>
       </c>
       <c r="H37" s="2" t="n">
-        <v>1.84</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38">
@@ -7097,19 +7097,19 @@
         <v>36</v>
       </c>
       <c r="D38" s="2" t="n">
-        <v>19472</v>
+        <v>40000</v>
       </c>
       <c r="E38" s="2" t="n">
-        <v>393</v>
+        <v>0</v>
       </c>
       <c r="F38" s="2" t="n">
-        <v>52.27</v>
+        <v>0</v>
       </c>
       <c r="G38" s="2" t="n">
-        <v>0.04</v>
+        <v>0</v>
       </c>
       <c r="H38" s="2" t="n">
-        <v>1.88</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39">
@@ -7123,19 +7123,19 @@
         <v>37</v>
       </c>
       <c r="D39" s="2" t="n">
-        <v>19086</v>
+        <v>40000</v>
       </c>
       <c r="E39" s="2" t="n">
-        <v>386</v>
+        <v>0</v>
       </c>
       <c r="F39" s="2" t="n">
-        <v>51.34</v>
+        <v>0</v>
       </c>
       <c r="G39" s="2" t="n">
-        <v>0.04</v>
+        <v>0</v>
       </c>
       <c r="H39" s="2" t="n">
-        <v>1.92</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40">
@@ -7149,19 +7149,19 @@
         <v>38</v>
       </c>
       <c r="D40" s="2" t="n">
-        <v>18708</v>
+        <v>40000</v>
       </c>
       <c r="E40" s="2" t="n">
-        <v>378</v>
+        <v>0</v>
       </c>
       <c r="F40" s="2" t="n">
-        <v>50.27</v>
+        <v>0</v>
       </c>
       <c r="G40" s="2" t="n">
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="H40" s="2" t="n">
-        <v>1.95</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41">
@@ -7175,19 +7175,19 @@
         <v>39</v>
       </c>
       <c r="D41" s="2" t="n">
-        <v>18338</v>
+        <v>40000</v>
       </c>
       <c r="E41" s="2" t="n">
-        <v>370</v>
+        <v>0</v>
       </c>
       <c r="F41" s="2" t="n">
-        <v>49.21</v>
+        <v>0</v>
       </c>
       <c r="G41" s="2" t="n">
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="H41" s="2" t="n">
-        <v>1.98</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42">
@@ -7201,19 +7201,19 @@
         <v>40</v>
       </c>
       <c r="D42" s="2" t="n">
-        <v>17975</v>
+        <v>40000</v>
       </c>
       <c r="E42" s="2" t="n">
-        <v>363</v>
+        <v>0</v>
       </c>
       <c r="F42" s="2" t="n">
-        <v>48.28</v>
+        <v>0</v>
       </c>
       <c r="G42" s="2" t="n">
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="H42" s="2" t="n">
-        <v>2.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43">
@@ -7227,19 +7227,19 @@
         <v>41</v>
       </c>
       <c r="D43" s="2" t="n">
-        <v>17619</v>
+        <v>40000</v>
       </c>
       <c r="E43" s="2" t="n">
-        <v>356</v>
+        <v>0</v>
       </c>
       <c r="F43" s="2" t="n">
-        <v>47.35</v>
+        <v>0</v>
       </c>
       <c r="G43" s="2" t="n">
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="H43" s="2" t="n">
-        <v>2.04</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44">
@@ -7253,19 +7253,19 @@
         <v>42</v>
       </c>
       <c r="D44" s="2" t="n">
-        <v>17270</v>
+        <v>40000</v>
       </c>
       <c r="E44" s="2" t="n">
-        <v>349</v>
+        <v>0</v>
       </c>
       <c r="F44" s="2" t="n">
-        <v>46.42</v>
+        <v>0</v>
       </c>
       <c r="G44" s="2" t="n">
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="H44" s="2" t="n">
-        <v>2.07</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45">
@@ -7279,19 +7279,19 @@
         <v>43</v>
       </c>
       <c r="D45" s="2" t="n">
-        <v>16928</v>
+        <v>40000</v>
       </c>
       <c r="E45" s="2" t="n">
-        <v>342</v>
+        <v>0</v>
       </c>
       <c r="F45" s="2" t="n">
-        <v>45.49</v>
+        <v>0</v>
       </c>
       <c r="G45" s="2" t="n">
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="H45" s="2" t="n">
-        <v>2.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46">
@@ -7305,19 +7305,19 @@
         <v>44</v>
       </c>
       <c r="D46" s="2" t="n">
-        <v>16593</v>
+        <v>40000</v>
       </c>
       <c r="E46" s="2" t="n">
-        <v>335</v>
+        <v>0</v>
       </c>
       <c r="F46" s="2" t="n">
-        <v>44.56</v>
+        <v>0</v>
       </c>
       <c r="G46" s="2" t="n">
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="H46" s="2" t="n">
-        <v>2.13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47">
@@ -7331,19 +7331,19 @@
         <v>45</v>
       </c>
       <c r="D47" s="2" t="n">
-        <v>16264</v>
+        <v>40000</v>
       </c>
       <c r="E47" s="2" t="n">
-        <v>329</v>
+        <v>0</v>
       </c>
       <c r="F47" s="2" t="n">
-        <v>43.76</v>
+        <v>0</v>
       </c>
       <c r="G47" s="2" t="n">
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="H47" s="2" t="n">
-        <v>2.16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48">
@@ -7357,19 +7357,19 @@
         <v>46</v>
       </c>
       <c r="D48" s="2" t="n">
-        <v>15942</v>
+        <v>40000</v>
       </c>
       <c r="E48" s="2" t="n">
-        <v>322</v>
+        <v>0</v>
       </c>
       <c r="F48" s="2" t="n">
-        <v>42.83</v>
+        <v>0</v>
       </c>
       <c r="G48" s="2" t="n">
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="H48" s="2" t="n">
-        <v>2.19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49">
@@ -7383,19 +7383,19 @@
         <v>47</v>
       </c>
       <c r="D49" s="2" t="n">
-        <v>15627</v>
+        <v>40000</v>
       </c>
       <c r="E49" s="2" t="n">
-        <v>315</v>
+        <v>0</v>
       </c>
       <c r="F49" s="2" t="n">
-        <v>41.9</v>
+        <v>0</v>
       </c>
       <c r="G49" s="2" t="n">
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="H49" s="2" t="n">
-        <v>2.22</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50">
@@ -7409,19 +7409,19 @@
         <v>48</v>
       </c>
       <c r="D50" s="2" t="n">
-        <v>15317</v>
+        <v>40000</v>
       </c>
       <c r="E50" s="2" t="n">
-        <v>310</v>
+        <v>0</v>
       </c>
       <c r="F50" s="2" t="n">
-        <v>41.23</v>
+        <v>0</v>
       </c>
       <c r="G50" s="2" t="n">
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="H50" s="2" t="n">
-        <v>2.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51">
@@ -7435,19 +7435,19 @@
         <v>49</v>
       </c>
       <c r="D51" s="2" t="n">
-        <v>15014</v>
+        <v>40000</v>
       </c>
       <c r="E51" s="2" t="n">
-        <v>303</v>
+        <v>0</v>
       </c>
       <c r="F51" s="2" t="n">
-        <v>40.3</v>
+        <v>0</v>
       </c>
       <c r="G51" s="2" t="n">
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="H51" s="2" t="n">
-        <v>2.28</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52">
@@ -7461,19 +7461,19 @@
         <v>50</v>
       </c>
       <c r="D52" s="2" t="n">
-        <v>14717</v>
+        <v>40000</v>
       </c>
       <c r="E52" s="2" t="n">
-        <v>297</v>
+        <v>0</v>
       </c>
       <c r="F52" s="2" t="n">
-        <v>39.5</v>
+        <v>0</v>
       </c>
       <c r="G52" s="2" t="n">
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="H52" s="2" t="n">
-        <v>2.31</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53">
@@ -7487,19 +7487,19 @@
         <v>51</v>
       </c>
       <c r="D53" s="2" t="n">
-        <v>14425</v>
+        <v>40000</v>
       </c>
       <c r="E53" s="2" t="n">
-        <v>292</v>
+        <v>0</v>
       </c>
       <c r="F53" s="2" t="n">
-        <v>38.84</v>
+        <v>0</v>
       </c>
       <c r="G53" s="2" t="n">
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="H53" s="2" t="n">
-        <v>2.34</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54">
@@ -7513,19 +7513,19 @@
         <v>52</v>
       </c>
       <c r="D54" s="2" t="n">
-        <v>14140</v>
+        <v>40000</v>
       </c>
       <c r="E54" s="2" t="n">
-        <v>285</v>
+        <v>0</v>
       </c>
       <c r="F54" s="2" t="n">
-        <v>37.91</v>
+        <v>0</v>
       </c>
       <c r="G54" s="2" t="n">
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="H54" s="2" t="n">
-        <v>2.37</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -7615,19 +7615,19 @@
         <v>1</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>24505</v>
+        <v>26282</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>495</v>
+        <v>-1282</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>65.84</v>
+        <v>-170.51</v>
       </c>
       <c r="G3" s="2" t="n">
-        <v>0.05</v>
+        <v>-0.12</v>
       </c>
       <c r="H3" s="2" t="n">
-        <v>0.05</v>
+        <v>-0.12</v>
       </c>
     </row>
     <row r="4">
@@ -7641,19 +7641,19 @@
         <v>2</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>24020</v>
+        <v>27629</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>485</v>
+        <v>-1347</v>
       </c>
       <c r="F4" s="2" t="n">
-        <v>64.51</v>
+        <v>-179.15</v>
       </c>
       <c r="G4" s="2" t="n">
-        <v>0.04</v>
+        <v>-0.12</v>
       </c>
       <c r="H4" s="2" t="n">
-        <v>0.09</v>
+        <v>-0.24</v>
       </c>
     </row>
     <row r="5">
@@ -7667,19 +7667,19 @@
         <v>3</v>
       </c>
       <c r="D5" s="2" t="n">
-        <v>23544</v>
+        <v>29045</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>476</v>
+        <v>-1416</v>
       </c>
       <c r="F5" s="2" t="n">
-        <v>63.31</v>
+        <v>-188.33</v>
       </c>
       <c r="G5" s="2" t="n">
-        <v>0.04</v>
+        <v>-0.13</v>
       </c>
       <c r="H5" s="2" t="n">
-        <v>0.13</v>
+        <v>-0.37</v>
       </c>
     </row>
     <row r="6">
@@ -7693,19 +7693,19 @@
         <v>4</v>
       </c>
       <c r="D6" s="2" t="n">
-        <v>23078</v>
+        <v>30534</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>466</v>
+        <v>-1489</v>
       </c>
       <c r="F6" s="2" t="n">
-        <v>61.98</v>
+        <v>-198.04</v>
       </c>
       <c r="G6" s="2" t="n">
-        <v>0.04</v>
+        <v>-0.14</v>
       </c>
       <c r="H6" s="2" t="n">
-        <v>0.17</v>
+        <v>-0.51</v>
       </c>
     </row>
     <row r="7">
@@ -7719,19 +7719,19 @@
         <v>5</v>
       </c>
       <c r="D7" s="2" t="n">
-        <v>22621</v>
+        <v>32100</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>457</v>
+        <v>-1566</v>
       </c>
       <c r="F7" s="2" t="n">
-        <v>60.78</v>
+        <v>-208.28</v>
       </c>
       <c r="G7" s="2" t="n">
-        <v>0.04</v>
+        <v>-0.14</v>
       </c>
       <c r="H7" s="2" t="n">
-        <v>0.21</v>
+        <v>-0.65</v>
       </c>
     </row>
     <row r="8">
@@ -7745,19 +7745,19 @@
         <v>6</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>22173</v>
+        <v>33745</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>448</v>
+        <v>-1645</v>
       </c>
       <c r="F8" s="2" t="n">
-        <v>59.58</v>
+        <v>-218.79</v>
       </c>
       <c r="G8" s="2" t="n">
-        <v>0.04</v>
+        <v>-0.15</v>
       </c>
       <c r="H8" s="2" t="n">
-        <v>0.25</v>
+        <v>-0.8</v>
       </c>
     </row>
     <row r="9">
@@ -7771,19 +7771,19 @@
         <v>7</v>
       </c>
       <c r="D9" s="2" t="n">
-        <v>21734</v>
+        <v>35475</v>
       </c>
       <c r="E9" s="2" t="n">
-        <v>439</v>
+        <v>-1730</v>
       </c>
       <c r="F9" s="2" t="n">
-        <v>58.39</v>
+        <v>-230.09</v>
       </c>
       <c r="G9" s="2" t="n">
-        <v>0.04</v>
+        <v>-0.16</v>
       </c>
       <c r="H9" s="2" t="n">
-        <v>0.29</v>
+        <v>-0.96</v>
       </c>
     </row>
     <row r="10">
@@ -7797,19 +7797,19 @@
         <v>8</v>
       </c>
       <c r="D10" s="2" t="n">
-        <v>21304</v>
+        <v>37294</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>430</v>
+        <v>-1819</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>57.19</v>
+        <v>-241.93</v>
       </c>
       <c r="G10" s="2" t="n">
-        <v>0.04</v>
+        <v>-0.17</v>
       </c>
       <c r="H10" s="2" t="n">
-        <v>0.33</v>
+        <v>-1.13</v>
       </c>
     </row>
     <row r="11">
@@ -7823,19 +7823,19 @@
         <v>9</v>
       </c>
       <c r="D11" s="2" t="n">
-        <v>20882</v>
+        <v>39206</v>
       </c>
       <c r="E11" s="2" t="n">
-        <v>422</v>
+        <v>-1912</v>
       </c>
       <c r="F11" s="2" t="n">
-        <v>56.13</v>
+        <v>-254.3</v>
       </c>
       <c r="G11" s="2" t="n">
-        <v>0.04</v>
+        <v>-0.17</v>
       </c>
       <c r="H11" s="2" t="n">
-        <v>0.37</v>
+        <v>-1.3</v>
       </c>
     </row>
     <row r="12">
@@ -7849,19 +7849,19 @@
         <v>10</v>
       </c>
       <c r="D12" s="2" t="n">
-        <v>20469</v>
+        <v>41216</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>413</v>
+        <v>-2010</v>
       </c>
       <c r="F12" s="2" t="n">
-        <v>54.93</v>
+        <v>-267.33</v>
       </c>
       <c r="G12" s="2" t="n">
-        <v>0.04</v>
+        <v>-0.18</v>
       </c>
       <c r="H12" s="2" t="n">
-        <v>0.41</v>
+        <v>-1.48</v>
       </c>
     </row>
     <row r="13">
@@ -7875,19 +7875,19 @@
         <v>11</v>
       </c>
       <c r="D13" s="2" t="n">
-        <v>20063</v>
+        <v>43329</v>
       </c>
       <c r="E13" s="2" t="n">
-        <v>406</v>
+        <v>-2113</v>
       </c>
       <c r="F13" s="2" t="n">
-        <v>54</v>
+        <v>-281.03</v>
       </c>
       <c r="G13" s="2" t="n">
-        <v>0.04</v>
+        <v>-0.19</v>
       </c>
       <c r="H13" s="2" t="n">
-        <v>0.45</v>
+        <v>-1.67</v>
       </c>
     </row>
     <row r="14">
@@ -7901,19 +7901,19 @@
         <v>12</v>
       </c>
       <c r="D14" s="2" t="n">
-        <v>19666</v>
+        <v>45550</v>
       </c>
       <c r="E14" s="2" t="n">
-        <v>397</v>
+        <v>-2221</v>
       </c>
       <c r="F14" s="2" t="n">
-        <v>52.8</v>
+        <v>-295.39</v>
       </c>
       <c r="G14" s="2" t="n">
-        <v>0.04</v>
+        <v>-0.2</v>
       </c>
       <c r="H14" s="2" t="n">
-        <v>0.49</v>
+        <v>-1.87</v>
       </c>
     </row>
     <row r="15">
@@ -7927,19 +7927,19 @@
         <v>13</v>
       </c>
       <c r="D15" s="2" t="n">
-        <v>19277</v>
+        <v>47885</v>
       </c>
       <c r="E15" s="2" t="n">
-        <v>389</v>
+        <v>-2335</v>
       </c>
       <c r="F15" s="2" t="n">
-        <v>51.74</v>
+        <v>-310.56</v>
       </c>
       <c r="G15" s="2" t="n">
-        <v>0.04</v>
+        <v>-0.21</v>
       </c>
       <c r="H15" s="2" t="n">
-        <v>0.53</v>
+        <v>-2.08</v>
       </c>
     </row>
     <row r="16">
@@ -7953,19 +7953,19 @@
         <v>14</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>18895</v>
+        <v>50340</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>382</v>
+        <v>-2455</v>
       </c>
       <c r="F16" s="2" t="n">
-        <v>50.81</v>
+        <v>-326.52</v>
       </c>
       <c r="G16" s="2" t="n">
-        <v>0.03</v>
+        <v>-0.22</v>
       </c>
       <c r="H16" s="2" t="n">
-        <v>0.56</v>
+        <v>-2.3</v>
       </c>
     </row>
     <row r="17">
@@ -7979,19 +7979,19 @@
         <v>15</v>
       </c>
       <c r="D17" s="2" t="n">
-        <v>18521</v>
+        <v>52921</v>
       </c>
       <c r="E17" s="2" t="n">
-        <v>374</v>
+        <v>-2581</v>
       </c>
       <c r="F17" s="2" t="n">
-        <v>49.74</v>
+        <v>-343.27</v>
       </c>
       <c r="G17" s="2" t="n">
-        <v>0.03</v>
+        <v>-0.24</v>
       </c>
       <c r="H17" s="2" t="n">
-        <v>0.59</v>
+        <v>-2.54</v>
       </c>
     </row>
     <row r="18">
@@ -8005,19 +8005,19 @@
         <v>16</v>
       </c>
       <c r="D18" s="2" t="n">
-        <v>18154</v>
+        <v>55634</v>
       </c>
       <c r="E18" s="2" t="n">
-        <v>367</v>
+        <v>-2713</v>
       </c>
       <c r="F18" s="2" t="n">
-        <v>48.81</v>
+        <v>-360.83</v>
       </c>
       <c r="G18" s="2" t="n">
-        <v>0.03</v>
+        <v>-0.25</v>
       </c>
       <c r="H18" s="2" t="n">
-        <v>0.62</v>
+        <v>-2.79</v>
       </c>
     </row>
     <row r="19">
@@ -8031,19 +8031,19 @@
         <v>17</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>17795</v>
+        <v>58486</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>359</v>
+        <v>-2852</v>
       </c>
       <c r="F19" s="2" t="n">
-        <v>47.75</v>
+        <v>-379.32</v>
       </c>
       <c r="G19" s="2" t="n">
-        <v>0.03</v>
+        <v>-0.26</v>
       </c>
       <c r="H19" s="2" t="n">
-        <v>0.65</v>
+        <v>-3.05</v>
       </c>
     </row>
     <row r="20">
@@ -8057,19 +8057,19 @@
         <v>18</v>
       </c>
       <c r="D20" s="2" t="n">
-        <v>17443</v>
+        <v>61484</v>
       </c>
       <c r="E20" s="2" t="n">
-        <v>352</v>
+        <v>-2998</v>
       </c>
       <c r="F20" s="2" t="n">
-        <v>46.82</v>
+        <v>-398.73</v>
       </c>
       <c r="G20" s="2" t="n">
-        <v>0.03</v>
+        <v>-0.27</v>
       </c>
       <c r="H20" s="2" t="n">
-        <v>0.68</v>
+        <v>-3.32</v>
       </c>
     </row>
     <row r="21">
@@ -8083,19 +8083,19 @@
         <v>19</v>
       </c>
       <c r="D21" s="2" t="n">
-        <v>17097</v>
+        <v>64636</v>
       </c>
       <c r="E21" s="2" t="n">
-        <v>346</v>
+        <v>-3152</v>
       </c>
       <c r="F21" s="2" t="n">
-        <v>46.02</v>
+        <v>-419.22</v>
       </c>
       <c r="G21" s="2" t="n">
-        <v>0.03</v>
+        <v>-0.29</v>
       </c>
       <c r="H21" s="2" t="n">
-        <v>0.71</v>
+        <v>-3.61</v>
       </c>
     </row>
     <row r="22">
@@ -8109,19 +8109,19 @@
         <v>20</v>
       </c>
       <c r="D22" s="2" t="n">
-        <v>16759</v>
+        <v>67950</v>
       </c>
       <c r="E22" s="2" t="n">
-        <v>338</v>
+        <v>-3314</v>
       </c>
       <c r="F22" s="2" t="n">
-        <v>44.95</v>
+        <v>-440.76</v>
       </c>
       <c r="G22" s="2" t="n">
-        <v>0.03</v>
+        <v>-0.3</v>
       </c>
       <c r="H22" s="2" t="n">
-        <v>0.74</v>
+        <v>-3.91</v>
       </c>
     </row>
     <row r="23">
@@ -8135,19 +8135,19 @@
         <v>21</v>
       </c>
       <c r="D23" s="2" t="n">
-        <v>16427</v>
+        <v>71434</v>
       </c>
       <c r="E23" s="2" t="n">
-        <v>332</v>
+        <v>-3484</v>
       </c>
       <c r="F23" s="2" t="n">
-        <v>44.16</v>
+        <v>-463.37</v>
       </c>
       <c r="G23" s="2" t="n">
-        <v>0.03</v>
+        <v>-0.32</v>
       </c>
       <c r="H23" s="2" t="n">
-        <v>0.77</v>
+        <v>-4.23</v>
       </c>
     </row>
     <row r="24">
@@ -8161,19 +8161,19 @@
         <v>22</v>
       </c>
       <c r="D24" s="2" t="n">
-        <v>16102</v>
+        <v>75096</v>
       </c>
       <c r="E24" s="2" t="n">
-        <v>325</v>
+        <v>-3662</v>
       </c>
       <c r="F24" s="2" t="n">
-        <v>43.23</v>
+        <v>-487.05</v>
       </c>
       <c r="G24" s="2" t="n">
-        <v>0.03</v>
+        <v>-0.33</v>
       </c>
       <c r="H24" s="2" t="n">
-        <v>0.8</v>
+        <v>-4.56</v>
       </c>
     </row>
     <row r="25">
@@ -8187,19 +8187,19 @@
         <v>23</v>
       </c>
       <c r="D25" s="2" t="n">
-        <v>15783</v>
+        <v>78945</v>
       </c>
       <c r="E25" s="2" t="n">
-        <v>319</v>
+        <v>-3849</v>
       </c>
       <c r="F25" s="2" t="n">
-        <v>42.43</v>
+        <v>-511.92</v>
       </c>
       <c r="G25" s="2" t="n">
-        <v>0.03</v>
+        <v>-0.35</v>
       </c>
       <c r="H25" s="2" t="n">
-        <v>0.83</v>
+        <v>-4.91</v>
       </c>
     </row>
     <row r="26">
@@ -8213,19 +8213,19 @@
         <v>24</v>
       </c>
       <c r="D26" s="2" t="n">
-        <v>15470</v>
+        <v>82993</v>
       </c>
       <c r="E26" s="2" t="n">
-        <v>313</v>
+        <v>-4048</v>
       </c>
       <c r="F26" s="2" t="n">
-        <v>41.63</v>
+        <v>-538.38</v>
       </c>
       <c r="G26" s="2" t="n">
-        <v>0.03</v>
+        <v>-0.37</v>
       </c>
       <c r="H26" s="2" t="n">
-        <v>0.86</v>
+        <v>-5.28</v>
       </c>
     </row>
     <row r="27">
@@ -8239,19 +8239,19 @@
         <v>25</v>
       </c>
       <c r="D27" s="2" t="n">
-        <v>15164</v>
+        <v>87247</v>
       </c>
       <c r="E27" s="2" t="n">
-        <v>306</v>
+        <v>-4254</v>
       </c>
       <c r="F27" s="2" t="n">
-        <v>40.7</v>
+        <v>-565.78</v>
       </c>
       <c r="G27" s="2" t="n">
-        <v>0.03</v>
+        <v>-0.39</v>
       </c>
       <c r="H27" s="2" t="n">
-        <v>0.89</v>
+        <v>-5.67</v>
       </c>
     </row>
     <row r="28">
@@ -8265,19 +8265,19 @@
         <v>26</v>
       </c>
       <c r="D28" s="2" t="n">
-        <v>14864</v>
+        <v>91720</v>
       </c>
       <c r="E28" s="2" t="n">
-        <v>300</v>
+        <v>-4473</v>
       </c>
       <c r="F28" s="2" t="n">
-        <v>39.9</v>
+        <v>-594.91</v>
       </c>
       <c r="G28" s="2" t="n">
-        <v>0.03</v>
+        <v>-0.41</v>
       </c>
       <c r="H28" s="2" t="n">
-        <v>0.92</v>
+        <v>-6.08</v>
       </c>
     </row>
     <row r="29">
@@ -8291,19 +8291,19 @@
         <v>27</v>
       </c>
       <c r="D29" s="2" t="n">
-        <v>14570</v>
+        <v>96422</v>
       </c>
       <c r="E29" s="2" t="n">
-        <v>294</v>
+        <v>-4702</v>
       </c>
       <c r="F29" s="2" t="n">
-        <v>39.1</v>
+        <v>-625.37</v>
       </c>
       <c r="G29" s="2" t="n">
-        <v>0.03</v>
+        <v>-0.43</v>
       </c>
       <c r="H29" s="2" t="n">
-        <v>0.95</v>
+        <v>-6.51</v>
       </c>
     </row>
     <row r="30">
@@ -8317,19 +8317,19 @@
         <v>28</v>
       </c>
       <c r="D30" s="2" t="n">
-        <v>14281</v>
+        <v>101365</v>
       </c>
       <c r="E30" s="2" t="n">
-        <v>289</v>
+        <v>-4943</v>
       </c>
       <c r="F30" s="2" t="n">
-        <v>38.44</v>
+        <v>-657.42</v>
       </c>
       <c r="G30" s="2" t="n">
-        <v>0.03</v>
+        <v>-0.45</v>
       </c>
       <c r="H30" s="2" t="n">
-        <v>0.98</v>
+        <v>-6.96</v>
       </c>
     </row>
     <row r="31">
@@ -8343,19 +8343,19 @@
         <v>29</v>
       </c>
       <c r="D31" s="2" t="n">
-        <v>13998</v>
+        <v>106562</v>
       </c>
       <c r="E31" s="2" t="n">
-        <v>283</v>
+        <v>-5197</v>
       </c>
       <c r="F31" s="2" t="n">
-        <v>37.64</v>
+        <v>-691.2</v>
       </c>
       <c r="G31" s="2" t="n">
-        <v>0.03</v>
+        <v>-0.47</v>
       </c>
       <c r="H31" s="2" t="n">
-        <v>1.01</v>
+        <v>-7.43</v>
       </c>
     </row>
     <row r="32">
@@ -8369,19 +8369,19 @@
         <v>30</v>
       </c>
       <c r="D32" s="2" t="n">
-        <v>13721</v>
+        <v>112025</v>
       </c>
       <c r="E32" s="2" t="n">
-        <v>277</v>
+        <v>-5463</v>
       </c>
       <c r="F32" s="2" t="n">
-        <v>36.84</v>
+        <v>-726.58</v>
       </c>
       <c r="G32" s="2" t="n">
-        <v>0.03</v>
+        <v>-0.5</v>
       </c>
       <c r="H32" s="2" t="n">
-        <v>1.04</v>
+        <v>-7.93</v>
       </c>
     </row>
     <row r="33">
@@ -8395,19 +8395,19 @@
         <v>31</v>
       </c>
       <c r="D33" s="2" t="n">
-        <v>13449</v>
+        <v>117768</v>
       </c>
       <c r="E33" s="2" t="n">
-        <v>272</v>
+        <v>-5743</v>
       </c>
       <c r="F33" s="2" t="n">
-        <v>36.18</v>
+        <v>-763.82</v>
       </c>
       <c r="G33" s="2" t="n">
-        <v>0.02</v>
+        <v>-0.52</v>
       </c>
       <c r="H33" s="2" t="n">
-        <v>1.06</v>
+        <v>-8.45</v>
       </c>
     </row>
     <row r="34">
@@ -8421,19 +8421,19 @@
         <v>32</v>
       </c>
       <c r="D34" s="2" t="n">
-        <v>13183</v>
+        <v>123805</v>
       </c>
       <c r="E34" s="2" t="n">
-        <v>266</v>
+        <v>-6037</v>
       </c>
       <c r="F34" s="2" t="n">
-        <v>35.38</v>
+        <v>-802.92</v>
       </c>
       <c r="G34" s="2" t="n">
-        <v>0.02</v>
+        <v>-0.55</v>
       </c>
       <c r="H34" s="2" t="n">
-        <v>1.08</v>
+        <v>-9</v>
       </c>
     </row>
     <row r="35">
@@ -8447,19 +8447,19 @@
         <v>33</v>
       </c>
       <c r="D35" s="2" t="n">
-        <v>12922</v>
+        <v>130152</v>
       </c>
       <c r="E35" s="2" t="n">
-        <v>261</v>
+        <v>-6347</v>
       </c>
       <c r="F35" s="2" t="n">
-        <v>34.71</v>
+        <v>-844.15</v>
       </c>
       <c r="G35" s="2" t="n">
-        <v>0.02</v>
+        <v>-0.58</v>
       </c>
       <c r="H35" s="2" t="n">
-        <v>1.1</v>
+        <v>-9.58</v>
       </c>
     </row>
     <row r="36">
@@ -8473,19 +8473,19 @@
         <v>34</v>
       </c>
       <c r="D36" s="2" t="n">
-        <v>12666</v>
+        <v>136825</v>
       </c>
       <c r="E36" s="2" t="n">
-        <v>256</v>
+        <v>-6673</v>
       </c>
       <c r="F36" s="2" t="n">
-        <v>34.05</v>
+        <v>-887.51</v>
       </c>
       <c r="G36" s="2" t="n">
-        <v>0.02</v>
+        <v>-0.61</v>
       </c>
       <c r="H36" s="2" t="n">
-        <v>1.12</v>
+        <v>-10.19</v>
       </c>
     </row>
     <row r="37">
@@ -8499,19 +8499,19 @@
         <v>35</v>
       </c>
       <c r="D37" s="2" t="n">
-        <v>12416</v>
+        <v>143839</v>
       </c>
       <c r="E37" s="2" t="n">
-        <v>250</v>
+        <v>-7014</v>
       </c>
       <c r="F37" s="2" t="n">
-        <v>33.25</v>
+        <v>-932.86</v>
       </c>
       <c r="G37" s="2" t="n">
-        <v>0.02</v>
+        <v>-0.64</v>
       </c>
       <c r="H37" s="2" t="n">
-        <v>1.14</v>
+        <v>-10.83</v>
       </c>
     </row>
     <row r="38">
@@ -8525,19 +8525,19 @@
         <v>36</v>
       </c>
       <c r="D38" s="2" t="n">
-        <v>12170</v>
+        <v>151213</v>
       </c>
       <c r="E38" s="2" t="n">
-        <v>246</v>
+        <v>-7374</v>
       </c>
       <c r="F38" s="2" t="n">
-        <v>32.72</v>
+        <v>-980.74</v>
       </c>
       <c r="G38" s="2" t="n">
-        <v>0.02</v>
+        <v>-0.67</v>
       </c>
       <c r="H38" s="2" t="n">
-        <v>1.16</v>
+        <v>-11.5</v>
       </c>
     </row>
     <row r="39">
@@ -8551,19 +8551,19 @@
         <v>37</v>
       </c>
       <c r="D39" s="2" t="n">
-        <v>11929</v>
+        <v>158965</v>
       </c>
       <c r="E39" s="2" t="n">
-        <v>241</v>
+        <v>-7752</v>
       </c>
       <c r="F39" s="2" t="n">
-        <v>32.05</v>
+        <v>-1031.02</v>
       </c>
       <c r="G39" s="2" t="n">
-        <v>0.02</v>
+        <v>-0.71</v>
       </c>
       <c r="H39" s="2" t="n">
-        <v>1.18</v>
+        <v>-12.21</v>
       </c>
     </row>
     <row r="40">
@@ -8577,19 +8577,19 @@
         <v>38</v>
       </c>
       <c r="D40" s="2" t="n">
-        <v>11693</v>
+        <v>167114</v>
       </c>
       <c r="E40" s="2" t="n">
-        <v>236</v>
+        <v>-8149</v>
       </c>
       <c r="F40" s="2" t="n">
-        <v>31.39</v>
+        <v>-1083.82</v>
       </c>
       <c r="G40" s="2" t="n">
-        <v>0.02</v>
+        <v>-0.74</v>
       </c>
       <c r="H40" s="2" t="n">
-        <v>1.2</v>
+        <v>-12.95</v>
       </c>
     </row>
     <row r="41">
@@ -8603,19 +8603,19 @@
         <v>39</v>
       </c>
       <c r="D41" s="2" t="n">
-        <v>11461</v>
+        <v>175682</v>
       </c>
       <c r="E41" s="2" t="n">
-        <v>232</v>
+        <v>-8568</v>
       </c>
       <c r="F41" s="2" t="n">
-        <v>30.86</v>
+        <v>-1139.54</v>
       </c>
       <c r="G41" s="2" t="n">
-        <v>0.02</v>
+        <v>-0.78</v>
       </c>
       <c r="H41" s="2" t="n">
-        <v>1.22</v>
+        <v>-13.73</v>
       </c>
     </row>
     <row r="42">
@@ -8629,19 +8629,19 @@
         <v>40</v>
       </c>
       <c r="D42" s="2" t="n">
-        <v>11234</v>
+        <v>184688</v>
       </c>
       <c r="E42" s="2" t="n">
-        <v>227</v>
+        <v>-9006</v>
       </c>
       <c r="F42" s="2" t="n">
-        <v>30.19</v>
+        <v>-1197.8</v>
       </c>
       <c r="G42" s="2" t="n">
-        <v>0.02</v>
+        <v>-0.82</v>
       </c>
       <c r="H42" s="2" t="n">
-        <v>1.24</v>
+        <v>-14.55</v>
       </c>
     </row>
     <row r="43">
@@ -8655,19 +8655,19 @@
         <v>41</v>
       </c>
       <c r="D43" s="2" t="n">
-        <v>11012</v>
+        <v>194156</v>
       </c>
       <c r="E43" s="2" t="n">
-        <v>222</v>
+        <v>-9468</v>
       </c>
       <c r="F43" s="2" t="n">
-        <v>29.53</v>
+        <v>-1259.24</v>
       </c>
       <c r="G43" s="2" t="n">
-        <v>0.02</v>
+        <v>-0.86</v>
       </c>
       <c r="H43" s="2" t="n">
-        <v>1.26</v>
+        <v>-15.41</v>
       </c>
     </row>
     <row r="44">
@@ -8681,19 +8681,19 @@
         <v>42</v>
       </c>
       <c r="D44" s="2" t="n">
-        <v>10794</v>
+        <v>204110</v>
       </c>
       <c r="E44" s="2" t="n">
-        <v>218</v>
+        <v>-9954</v>
       </c>
       <c r="F44" s="2" t="n">
-        <v>28.99</v>
+        <v>-1323.88</v>
       </c>
       <c r="G44" s="2" t="n">
-        <v>0.02</v>
+        <v>-0.91</v>
       </c>
       <c r="H44" s="2" t="n">
-        <v>1.28</v>
+        <v>-16.32</v>
       </c>
     </row>
     <row r="45">
@@ -8707,19 +8707,19 @@
         <v>43</v>
       </c>
       <c r="D45" s="2" t="n">
-        <v>10580</v>
+        <v>214574</v>
       </c>
       <c r="E45" s="2" t="n">
-        <v>214</v>
+        <v>-10464</v>
       </c>
       <c r="F45" s="2" t="n">
-        <v>28.46</v>
+        <v>-1391.71</v>
       </c>
       <c r="G45" s="2" t="n">
-        <v>0.02</v>
+        <v>-0.96</v>
       </c>
       <c r="H45" s="2" t="n">
-        <v>1.3</v>
+        <v>-17.28</v>
       </c>
     </row>
     <row r="46">
@@ -8733,19 +8733,19 @@
         <v>44</v>
       </c>
       <c r="D46" s="2" t="n">
-        <v>10371</v>
+        <v>225574</v>
       </c>
       <c r="E46" s="2" t="n">
-        <v>209</v>
+        <v>-11000</v>
       </c>
       <c r="F46" s="2" t="n">
-        <v>27.8</v>
+        <v>-1463</v>
       </c>
       <c r="G46" s="2" t="n">
-        <v>0.02</v>
+        <v>-1</v>
       </c>
       <c r="H46" s="2" t="n">
-        <v>1.32</v>
+        <v>-18.28</v>
       </c>
     </row>
     <row r="47">
@@ -8759,19 +8759,19 @@
         <v>45</v>
       </c>
       <c r="D47" s="2" t="n">
-        <v>10165</v>
+        <v>237138</v>
       </c>
       <c r="E47" s="2" t="n">
-        <v>206</v>
+        <v>-11564</v>
       </c>
       <c r="F47" s="2" t="n">
-        <v>27.4</v>
+        <v>-1538.01</v>
       </c>
       <c r="G47" s="2" t="n">
-        <v>0.02</v>
+        <v>-1.06</v>
       </c>
       <c r="H47" s="2" t="n">
-        <v>1.34</v>
+        <v>-19.34</v>
       </c>
     </row>
     <row r="48">
@@ -8785,19 +8785,19 @@
         <v>46</v>
       </c>
       <c r="D48" s="2" t="n">
-        <v>9964</v>
+        <v>249295</v>
       </c>
       <c r="E48" s="2" t="n">
-        <v>201</v>
+        <v>-12157</v>
       </c>
       <c r="F48" s="2" t="n">
-        <v>26.73</v>
+        <v>-1616.88</v>
       </c>
       <c r="G48" s="2" t="n">
-        <v>0.02</v>
+        <v>-1.11</v>
       </c>
       <c r="H48" s="2" t="n">
-        <v>1.36</v>
+        <v>-20.45</v>
       </c>
     </row>
     <row r="49">
@@ -8811,19 +8811,19 @@
         <v>47</v>
       </c>
       <c r="D49" s="2" t="n">
-        <v>9767</v>
+        <v>262075</v>
       </c>
       <c r="E49" s="2" t="n">
-        <v>197</v>
+        <v>-12780</v>
       </c>
       <c r="F49" s="2" t="n">
-        <v>26.2</v>
+        <v>-1699.74</v>
       </c>
       <c r="G49" s="2" t="n">
-        <v>0.02</v>
+        <v>-1.17</v>
       </c>
       <c r="H49" s="2" t="n">
-        <v>1.38</v>
+        <v>-21.62</v>
       </c>
     </row>
     <row r="50">
@@ -8837,19 +8837,19 @@
         <v>48</v>
       </c>
       <c r="D50" s="2" t="n">
-        <v>9573</v>
+        <v>275511</v>
       </c>
       <c r="E50" s="2" t="n">
-        <v>194</v>
+        <v>-13436</v>
       </c>
       <c r="F50" s="2" t="n">
-        <v>25.8</v>
+        <v>-1786.99</v>
       </c>
       <c r="G50" s="2" t="n">
-        <v>0.02</v>
+        <v>-1.23</v>
       </c>
       <c r="H50" s="2" t="n">
-        <v>1.4</v>
+        <v>-22.85</v>
       </c>
     </row>
     <row r="51">
@@ -8863,19 +8863,19 @@
         <v>49</v>
       </c>
       <c r="D51" s="2" t="n">
-        <v>9384</v>
+        <v>289635</v>
       </c>
       <c r="E51" s="2" t="n">
-        <v>189</v>
+        <v>-14124</v>
       </c>
       <c r="F51" s="2" t="n">
-        <v>25.14</v>
+        <v>-1878.49</v>
       </c>
       <c r="G51" s="2" t="n">
-        <v>0.02</v>
+        <v>-1.29</v>
       </c>
       <c r="H51" s="2" t="n">
-        <v>1.42</v>
+        <v>-24.14</v>
       </c>
     </row>
     <row r="52">
@@ -8889,19 +8889,19 @@
         <v>50</v>
       </c>
       <c r="D52" s="2" t="n">
-        <v>9198</v>
+        <v>304483</v>
       </c>
       <c r="E52" s="2" t="n">
-        <v>186</v>
+        <v>-14848</v>
       </c>
       <c r="F52" s="2" t="n">
-        <v>24.74</v>
+        <v>-1974.78</v>
       </c>
       <c r="G52" s="2" t="n">
-        <v>0.02</v>
+        <v>-1.36</v>
       </c>
       <c r="H52" s="2" t="n">
-        <v>1.44</v>
+        <v>-25.5</v>
       </c>
     </row>
     <row r="53">
@@ -8915,19 +8915,19 @@
         <v>51</v>
       </c>
       <c r="D53" s="2" t="n">
-        <v>9016</v>
+        <v>320093</v>
       </c>
       <c r="E53" s="2" t="n">
-        <v>182</v>
+        <v>-15610</v>
       </c>
       <c r="F53" s="2" t="n">
-        <v>24.21</v>
+        <v>-2076.13</v>
       </c>
       <c r="G53" s="2" t="n">
-        <v>0.02</v>
+        <v>-1.43</v>
       </c>
       <c r="H53" s="2" t="n">
-        <v>1.46</v>
+        <v>-26.93</v>
       </c>
     </row>
     <row r="54">
@@ -8941,19 +8941,19 @@
         <v>52</v>
       </c>
       <c r="D54" s="2" t="n">
-        <v>8837</v>
+        <v>336503</v>
       </c>
       <c r="E54" s="2" t="n">
-        <v>179</v>
+        <v>-16410</v>
       </c>
       <c r="F54" s="2" t="n">
-        <v>23.81</v>
+        <v>-2182.53</v>
       </c>
       <c r="G54" s="2" t="n">
-        <v>0.02</v>
+        <v>-1.5</v>
       </c>
       <c r="H54" s="2" t="n">
-        <v>1.48</v>
+        <v>-28.43</v>
       </c>
     </row>
   </sheetData>
@@ -9023,19 +9023,19 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>455793</v>
+        <v>458362</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>9207</v>
+        <v>6638</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>1093.86</v>
+        <v>752.17</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>0.75</v>
+        <v>0.51</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>0.75</v>
+        <v>0.51</v>
       </c>
     </row>
     <row r="4">
@@ -9043,19 +9043,19 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="n">
-        <v>446768</v>
+        <v>451945</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>9025</v>
+        <v>6417</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>1072.23</v>
+        <v>725.36</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>0.73</v>
+        <v>0.5</v>
       </c>
       <c r="F4" s="2" t="n">
-        <v>1.48</v>
+        <v>1.01</v>
       </c>
     </row>
     <row r="5">
@@ -9063,19 +9063,19 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="n">
-        <v>437923</v>
+        <v>445753</v>
       </c>
       <c r="C5" s="2" t="n">
-        <v>8845</v>
+        <v>6192</v>
       </c>
       <c r="D5" s="2" t="n">
-        <v>1050.85</v>
+        <v>698</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>0.72</v>
+        <v>0.48</v>
       </c>
       <c r="F5" s="2" t="n">
-        <v>2.2</v>
+        <v>1.49</v>
       </c>
     </row>
     <row r="6">
@@ -9083,19 +9083,19 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="n">
-        <v>429252</v>
+        <v>439783</v>
       </c>
       <c r="C6" s="2" t="n">
-        <v>8671</v>
+        <v>5970</v>
       </c>
       <c r="D6" s="2" t="n">
-        <v>1030.17</v>
+        <v>670.93</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>0.71</v>
+        <v>0.46</v>
       </c>
       <c r="F6" s="2" t="n">
-        <v>2.91</v>
+        <v>1.95</v>
       </c>
     </row>
     <row r="7">
@@ -9103,19 +9103,19 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="n">
-        <v>420755</v>
+        <v>434040</v>
       </c>
       <c r="C7" s="2" t="n">
-        <v>8497</v>
+        <v>5743</v>
       </c>
       <c r="D7" s="2" t="n">
-        <v>1009.52</v>
+        <v>643.24</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>0.69</v>
+        <v>0.44</v>
       </c>
       <c r="F7" s="2" t="n">
-        <v>3.6</v>
+        <v>2.39</v>
       </c>
     </row>
     <row r="8">
@@ -9123,19 +9123,19 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="n">
-        <v>412423</v>
+        <v>428518</v>
       </c>
       <c r="C8" s="2" t="n">
-        <v>8332</v>
+        <v>5522</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>989.88</v>
+        <v>616.15</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>0.68</v>
+        <v>0.42</v>
       </c>
       <c r="F8" s="2" t="n">
-        <v>4.28</v>
+        <v>2.81</v>
       </c>
     </row>
     <row r="9">
@@ -9143,19 +9143,19 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="n">
-        <v>404258</v>
+        <v>423224</v>
       </c>
       <c r="C9" s="2" t="n">
-        <v>8165</v>
+        <v>5294</v>
       </c>
       <c r="D9" s="2" t="n">
-        <v>970.05</v>
+        <v>588.2</v>
       </c>
       <c r="E9" s="2" t="n">
-        <v>0.66</v>
+        <v>0.4</v>
       </c>
       <c r="F9" s="2" t="n">
-        <v>4.94</v>
+        <v>3.21</v>
       </c>
     </row>
     <row r="10">
@@ -9163,19 +9163,19 @@
         <v>8</v>
       </c>
       <c r="B10" s="2" t="n">
-        <v>396254</v>
+        <v>418158</v>
       </c>
       <c r="C10" s="2" t="n">
-        <v>8004</v>
+        <v>5066</v>
       </c>
       <c r="D10" s="2" t="n">
-        <v>950.95</v>
+        <v>560.19</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>0.66</v>
+        <v>0.39</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>5.6</v>
+        <v>3.6</v>
       </c>
     </row>
     <row r="11">
@@ -9183,19 +9183,19 @@
         <v>9</v>
       </c>
       <c r="B11" s="2" t="n">
-        <v>388408</v>
+        <v>413321</v>
       </c>
       <c r="C11" s="2" t="n">
-        <v>7846</v>
+        <v>4837</v>
       </c>
       <c r="D11" s="2" t="n">
-        <v>932.18</v>
+        <v>531.97</v>
       </c>
       <c r="E11" s="2" t="n">
-        <v>0.63</v>
+        <v>0.36</v>
       </c>
       <c r="F11" s="2" t="n">
-        <v>6.23</v>
+        <v>3.96</v>
       </c>
     </row>
     <row r="12">
@@ -9203,19 +9203,19 @@
         <v>10</v>
       </c>
       <c r="B12" s="2" t="n">
-        <v>380719</v>
+        <v>408716</v>
       </c>
       <c r="C12" s="2" t="n">
-        <v>7689</v>
+        <v>4605</v>
       </c>
       <c r="D12" s="2" t="n">
-        <v>913.47</v>
+        <v>503.3</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>0.63</v>
+        <v>0.35</v>
       </c>
       <c r="F12" s="2" t="n">
-        <v>6.86</v>
+        <v>4.31</v>
       </c>
     </row>
     <row r="13">
@@ -9223,19 +9223,19 @@
         <v>11</v>
       </c>
       <c r="B13" s="2" t="n">
-        <v>373179</v>
+        <v>404344</v>
       </c>
       <c r="C13" s="2" t="n">
-        <v>7540</v>
+        <v>4372</v>
       </c>
       <c r="D13" s="2" t="n">
-        <v>895.84</v>
+        <v>474.49</v>
       </c>
       <c r="E13" s="2" t="n">
-        <v>0.62</v>
+        <v>0.33</v>
       </c>
       <c r="F13" s="2" t="n">
-        <v>7.48</v>
+        <v>4.64</v>
       </c>
     </row>
     <row r="14">
@@ -9243,19 +9243,19 @@
         <v>12</v>
       </c>
       <c r="B14" s="2" t="n">
-        <v>365792</v>
+        <v>400210</v>
       </c>
       <c r="C14" s="2" t="n">
-        <v>7387</v>
+        <v>4134</v>
       </c>
       <c r="D14" s="2" t="n">
-        <v>877.6</v>
+        <v>444.95</v>
       </c>
       <c r="E14" s="2" t="n">
-        <v>0.61</v>
+        <v>0.31</v>
       </c>
       <c r="F14" s="2" t="n">
-        <v>8.09</v>
+        <v>4.95</v>
       </c>
     </row>
     <row r="15">
@@ -9263,19 +9263,19 @@
         <v>13</v>
       </c>
       <c r="B15" s="2" t="n">
-        <v>358549</v>
+        <v>396314</v>
       </c>
       <c r="C15" s="2" t="n">
-        <v>7243</v>
+        <v>3896</v>
       </c>
       <c r="D15" s="2" t="n">
-        <v>860.5</v>
+        <v>415.34</v>
       </c>
       <c r="E15" s="2" t="n">
-        <v>0.59</v>
+        <v>0.28</v>
       </c>
       <c r="F15" s="2" t="n">
-        <v>8.68</v>
+        <v>5.23</v>
       </c>
     </row>
     <row r="16">
@@ -9283,19 +9283,19 @@
         <v>14</v>
       </c>
       <c r="B16" s="2" t="n">
-        <v>351450</v>
+        <v>392663</v>
       </c>
       <c r="C16" s="2" t="n">
-        <v>7099</v>
+        <v>3651</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>843.46</v>
+        <v>384.87</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>0.58</v>
+        <v>0.27</v>
       </c>
       <c r="F16" s="2" t="n">
-        <v>9.26</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="17">
@@ -9303,19 +9303,19 @@
         <v>15</v>
       </c>
       <c r="B17" s="2" t="n">
-        <v>344491</v>
+        <v>389257</v>
       </c>
       <c r="C17" s="2" t="n">
-        <v>6959</v>
+        <v>3406</v>
       </c>
       <c r="D17" s="2" t="n">
-        <v>826.74</v>
+        <v>354.2</v>
       </c>
       <c r="E17" s="2" t="n">
-        <v>0.56</v>
+        <v>0.24</v>
       </c>
       <c r="F17" s="2" t="n">
-        <v>9.82</v>
+        <v>5.74</v>
       </c>
     </row>
     <row r="18">
@@ -9323,19 +9323,19 @@
         <v>16</v>
       </c>
       <c r="B18" s="2" t="n">
-        <v>337670</v>
+        <v>386103</v>
       </c>
       <c r="C18" s="2" t="n">
-        <v>6821</v>
+        <v>3154</v>
       </c>
       <c r="D18" s="2" t="n">
-        <v>810.37</v>
+        <v>322.66</v>
       </c>
       <c r="E18" s="2" t="n">
-        <v>0.55</v>
+        <v>0.22</v>
       </c>
       <c r="F18" s="2" t="n">
-        <v>10.37</v>
+        <v>5.96</v>
       </c>
     </row>
     <row r="19">
@@ -9343,19 +9343,19 @@
         <v>17</v>
       </c>
       <c r="B19" s="2" t="n">
-        <v>330986</v>
+        <v>383205</v>
       </c>
       <c r="C19" s="2" t="n">
-        <v>6684</v>
+        <v>2898</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>794.14</v>
+        <v>290.59</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>0.55</v>
+        <v>0.21</v>
       </c>
       <c r="F19" s="2" t="n">
-        <v>10.92</v>
+        <v>6.17</v>
       </c>
     </row>
     <row r="20">
@@ -9363,19 +9363,19 @@
         <v>18</v>
       </c>
       <c r="B20" s="2" t="n">
-        <v>324431</v>
+        <v>380564</v>
       </c>
       <c r="C20" s="2" t="n">
-        <v>6555</v>
+        <v>2641</v>
       </c>
       <c r="D20" s="2" t="n">
-        <v>778.75</v>
+        <v>258.19</v>
       </c>
       <c r="E20" s="2" t="n">
-        <v>0.52</v>
+        <v>0.17</v>
       </c>
       <c r="F20" s="2" t="n">
-        <v>11.44</v>
+        <v>6.34</v>
       </c>
     </row>
     <row r="21">
@@ -9383,19 +9383,19 @@
         <v>19</v>
       </c>
       <c r="B21" s="2" t="n">
-        <v>318009</v>
+        <v>378192</v>
       </c>
       <c r="C21" s="2" t="n">
-        <v>6422</v>
+        <v>2372</v>
       </c>
       <c r="D21" s="2" t="n">
-        <v>762.98</v>
+        <v>224.32</v>
       </c>
       <c r="E21" s="2" t="n">
-        <v>0.52</v>
+        <v>0.15</v>
       </c>
       <c r="F21" s="2" t="n">
-        <v>11.96</v>
+        <v>6.49</v>
       </c>
     </row>
     <row r="22">
@@ -9403,19 +9403,19 @@
         <v>20</v>
       </c>
       <c r="B22" s="2" t="n">
-        <v>311713</v>
+        <v>376090</v>
       </c>
       <c r="C22" s="2" t="n">
-        <v>6296</v>
+        <v>2102</v>
       </c>
       <c r="D22" s="2" t="n">
-        <v>748</v>
+        <v>190.2</v>
       </c>
       <c r="E22" s="2" t="n">
-        <v>0.51</v>
+        <v>0.13</v>
       </c>
       <c r="F22" s="2" t="n">
-        <v>12.47</v>
+        <v>6.62</v>
       </c>
     </row>
     <row r="23">
@@ -9423,19 +9423,19 @@
         <v>21</v>
       </c>
       <c r="B23" s="2" t="n">
-        <v>305541</v>
+        <v>374265</v>
       </c>
       <c r="C23" s="2" t="n">
-        <v>6172</v>
+        <v>1825</v>
       </c>
       <c r="D23" s="2" t="n">
-        <v>733.3</v>
+        <v>155.15</v>
       </c>
       <c r="E23" s="2" t="n">
-        <v>0.51</v>
+        <v>0.11</v>
       </c>
       <c r="F23" s="2" t="n">
-        <v>12.98</v>
+        <v>6.73</v>
       </c>
     </row>
     <row r="24">
@@ -9443,19 +9443,19 @@
         <v>22</v>
       </c>
       <c r="B24" s="2" t="n">
-        <v>299492</v>
+        <v>372723</v>
       </c>
       <c r="C24" s="2" t="n">
-        <v>6049</v>
+        <v>1542</v>
       </c>
       <c r="D24" s="2" t="n">
-        <v>718.65</v>
+        <v>119.21</v>
       </c>
       <c r="E24" s="2" t="n">
-        <v>0.5</v>
+        <v>0.09</v>
       </c>
       <c r="F24" s="2" t="n">
-        <v>13.48</v>
+        <v>6.82</v>
       </c>
     </row>
     <row r="25">
@@ -9463,19 +9463,19 @@
         <v>23</v>
       </c>
       <c r="B25" s="2" t="n">
-        <v>293561</v>
+        <v>371470</v>
       </c>
       <c r="C25" s="2" t="n">
-        <v>5931</v>
+        <v>1253</v>
       </c>
       <c r="D25" s="2" t="n">
-        <v>704.61</v>
+        <v>82.43</v>
       </c>
       <c r="E25" s="2" t="n">
-        <v>0.49</v>
+        <v>0.06</v>
       </c>
       <c r="F25" s="2" t="n">
-        <v>13.97</v>
+        <v>6.88</v>
       </c>
     </row>
     <row r="26">
@@ -9483,19 +9483,19 @@
         <v>24</v>
       </c>
       <c r="B26" s="2" t="n">
-        <v>287748</v>
+        <v>370518</v>
       </c>
       <c r="C26" s="2" t="n">
-        <v>5813</v>
+        <v>952</v>
       </c>
       <c r="D26" s="2" t="n">
-        <v>690.63</v>
+        <v>44.12</v>
       </c>
       <c r="E26" s="2" t="n">
-        <v>0.48</v>
+        <v>0.03</v>
       </c>
       <c r="F26" s="2" t="n">
-        <v>14.45</v>
+        <v>6.91</v>
       </c>
     </row>
     <row r="27">
@@ -9503,19 +9503,19 @@
         <v>25</v>
       </c>
       <c r="B27" s="2" t="n">
-        <v>282050</v>
+        <v>369871</v>
       </c>
       <c r="C27" s="2" t="n">
-        <v>5698</v>
+        <v>647</v>
       </c>
       <c r="D27" s="2" t="n">
-        <v>676.99</v>
+        <v>5.21000000000001</v>
       </c>
       <c r="E27" s="2" t="n">
-        <v>0.46</v>
+        <v>-0.0000000000000000277555756156289</v>
       </c>
       <c r="F27" s="2" t="n">
-        <v>14.91</v>
+        <v>6.91</v>
       </c>
     </row>
     <row r="28">
@@ -9523,19 +9523,19 @@
         <v>26</v>
       </c>
       <c r="B28" s="2" t="n">
-        <v>276466</v>
+        <v>369540</v>
       </c>
       <c r="C28" s="2" t="n">
-        <v>5584</v>
+        <v>331</v>
       </c>
       <c r="D28" s="2" t="n">
-        <v>663.4</v>
+        <v>-35.25</v>
       </c>
       <c r="E28" s="2" t="n">
-        <v>0.46</v>
+        <v>-0.02</v>
       </c>
       <c r="F28" s="2" t="n">
-        <v>15.37</v>
+        <v>6.89</v>
       </c>
     </row>
     <row r="29">
@@ -9543,19 +9543,19 @@
         <v>27</v>
       </c>
       <c r="B29" s="2" t="n">
-        <v>270993</v>
+        <v>369534</v>
       </c>
       <c r="C29" s="2" t="n">
-        <v>5473</v>
+        <v>6</v>
       </c>
       <c r="D29" s="2" t="n">
-        <v>650.23</v>
+        <v>-76.88</v>
       </c>
       <c r="E29" s="2" t="n">
-        <v>0.45</v>
+        <v>-0.05</v>
       </c>
       <c r="F29" s="2" t="n">
-        <v>15.82</v>
+        <v>6.84</v>
       </c>
     </row>
     <row r="30">
@@ -9563,19 +9563,19 @@
         <v>28</v>
       </c>
       <c r="B30" s="2" t="n">
-        <v>265627</v>
+        <v>369861</v>
       </c>
       <c r="C30" s="2" t="n">
-        <v>5366</v>
+        <v>-327</v>
       </c>
       <c r="D30" s="2" t="n">
-        <v>637.52</v>
+        <v>-119.65</v>
       </c>
       <c r="E30" s="2" t="n">
-        <v>0.44</v>
+        <v>-0.08</v>
       </c>
       <c r="F30" s="2" t="n">
-        <v>16.26</v>
+        <v>6.76</v>
       </c>
     </row>
     <row r="31">
@@ -9583,19 +9583,19 @@
         <v>29</v>
       </c>
       <c r="B31" s="2" t="n">
-        <v>260368</v>
+        <v>370535</v>
       </c>
       <c r="C31" s="2" t="n">
-        <v>5259</v>
+        <v>-674</v>
       </c>
       <c r="D31" s="2" t="n">
-        <v>624.8</v>
+        <v>-164.29</v>
       </c>
       <c r="E31" s="2" t="n">
-        <v>0.42</v>
+        <v>-0.12</v>
       </c>
       <c r="F31" s="2" t="n">
-        <v>16.68</v>
+        <v>6.64</v>
       </c>
     </row>
     <row r="32">
@@ -9603,19 +9603,19 @@
         <v>30</v>
       </c>
       <c r="B32" s="2" t="n">
-        <v>255214</v>
+        <v>371564</v>
       </c>
       <c r="C32" s="2" t="n">
-        <v>5154</v>
+        <v>-1029</v>
       </c>
       <c r="D32" s="2" t="n">
-        <v>612.35</v>
+        <v>-209.99</v>
       </c>
       <c r="E32" s="2" t="n">
-        <v>0.42</v>
+        <v>-0.15</v>
       </c>
       <c r="F32" s="2" t="n">
-        <v>17.1</v>
+        <v>6.49</v>
       </c>
     </row>
     <row r="33">
@@ -9623,19 +9623,19 @@
         <v>31</v>
       </c>
       <c r="B33" s="2" t="n">
-        <v>250159</v>
+        <v>372959</v>
       </c>
       <c r="C33" s="2" t="n">
-        <v>5055</v>
+        <v>-1395</v>
       </c>
       <c r="D33" s="2" t="n">
-        <v>600.58</v>
+        <v>-257.28</v>
       </c>
       <c r="E33" s="2" t="n">
-        <v>0.41</v>
+        <v>-0.17</v>
       </c>
       <c r="F33" s="2" t="n">
-        <v>17.51</v>
+        <v>6.32</v>
       </c>
     </row>
     <row r="34">
@@ -9643,19 +9643,19 @@
         <v>32</v>
       </c>
       <c r="B34" s="2" t="n">
-        <v>245207</v>
+        <v>374736</v>
       </c>
       <c r="C34" s="2" t="n">
-        <v>4952</v>
+        <v>-1777</v>
       </c>
       <c r="D34" s="2" t="n">
-        <v>588.34</v>
+        <v>-306.62</v>
       </c>
       <c r="E34" s="2" t="n">
-        <v>0.41</v>
+        <v>-0.2</v>
       </c>
       <c r="F34" s="2" t="n">
-        <v>17.92</v>
+        <v>6.12</v>
       </c>
     </row>
     <row r="35">
@@ -9663,19 +9663,19 @@
         <v>33</v>
       </c>
       <c r="B35" s="2" t="n">
-        <v>240352</v>
+        <v>376907</v>
       </c>
       <c r="C35" s="2" t="n">
-        <v>4855</v>
+        <v>-2171</v>
       </c>
       <c r="D35" s="2" t="n">
-        <v>576.81</v>
+        <v>-357.64</v>
       </c>
       <c r="E35" s="2" t="n">
-        <v>0.4</v>
+        <v>-0.24</v>
       </c>
       <c r="F35" s="2" t="n">
-        <v>18.32</v>
+        <v>5.88</v>
       </c>
     </row>
     <row r="36">
@@ -9683,19 +9683,19 @@
         <v>34</v>
       </c>
       <c r="B36" s="2" t="n">
-        <v>235592</v>
+        <v>379485</v>
       </c>
       <c r="C36" s="2" t="n">
-        <v>4760</v>
+        <v>-2578</v>
       </c>
       <c r="D36" s="2" t="n">
-        <v>565.5</v>
+        <v>-410.46</v>
       </c>
       <c r="E36" s="2" t="n">
-        <v>0.38</v>
+        <v>-0.29</v>
       </c>
       <c r="F36" s="2" t="n">
-        <v>18.7</v>
+        <v>5.59</v>
       </c>
     </row>
     <row r="37">
@@ -9703,19 +9703,19 @@
         <v>35</v>
       </c>
       <c r="B37" s="2" t="n">
-        <v>230930</v>
+        <v>382488</v>
       </c>
       <c r="C37" s="2" t="n">
-        <v>4662</v>
+        <v>-3003</v>
       </c>
       <c r="D37" s="2" t="n">
-        <v>553.85</v>
+        <v>-465.59</v>
       </c>
       <c r="E37" s="2" t="n">
-        <v>0.38</v>
+        <v>-0.32</v>
       </c>
       <c r="F37" s="2" t="n">
-        <v>19.08</v>
+        <v>5.27</v>
       </c>
     </row>
     <row r="38">
@@ -9723,19 +9723,19 @@
         <v>36</v>
       </c>
       <c r="B38" s="2" t="n">
-        <v>226358</v>
+        <v>385929</v>
       </c>
       <c r="C38" s="2" t="n">
-        <v>4572</v>
+        <v>-3441</v>
       </c>
       <c r="D38" s="2" t="n">
-        <v>543.2</v>
+        <v>-522.53</v>
       </c>
       <c r="E38" s="2" t="n">
-        <v>0.38</v>
+        <v>-0.35</v>
       </c>
       <c r="F38" s="2" t="n">
-        <v>19.46</v>
+        <v>4.92</v>
       </c>
     </row>
     <row r="39">
@@ -9743,19 +9743,19 @@
         <v>37</v>
       </c>
       <c r="B39" s="2" t="n">
-        <v>221875</v>
+        <v>389825</v>
       </c>
       <c r="C39" s="2" t="n">
-        <v>4483</v>
+        <v>-3896</v>
       </c>
       <c r="D39" s="2" t="n">
-        <v>532.61</v>
+        <v>-581.8</v>
       </c>
       <c r="E39" s="2" t="n">
-        <v>0.37</v>
+        <v>-0.4</v>
       </c>
       <c r="F39" s="2" t="n">
-        <v>19.83</v>
+        <v>4.52</v>
       </c>
     </row>
     <row r="40">
@@ -9763,19 +9763,19 @@
         <v>38</v>
       </c>
       <c r="B40" s="2" t="n">
-        <v>217481</v>
+        <v>394194</v>
       </c>
       <c r="C40" s="2" t="n">
-        <v>4394</v>
+        <v>-4369</v>
       </c>
       <c r="D40" s="2" t="n">
-        <v>522.03</v>
+        <v>-643.45</v>
       </c>
       <c r="E40" s="2" t="n">
-        <v>0.35</v>
+        <v>-0.44</v>
       </c>
       <c r="F40" s="2" t="n">
-        <v>20.18</v>
+        <v>4.08</v>
       </c>
     </row>
     <row r="41">
@@ -9783,19 +9783,19 @@
         <v>39</v>
       </c>
       <c r="B41" s="2" t="n">
-        <v>213175</v>
+        <v>399058</v>
       </c>
       <c r="C41" s="2" t="n">
-        <v>4306</v>
+        <v>-4864</v>
       </c>
       <c r="D41" s="2" t="n">
-        <v>511.58</v>
+        <v>-708.03</v>
       </c>
       <c r="E41" s="2" t="n">
-        <v>0.34</v>
+        <v>-0.49</v>
       </c>
       <c r="F41" s="2" t="n">
-        <v>20.52</v>
+        <v>3.59</v>
       </c>
     </row>
     <row r="42">
@@ -9803,19 +9803,19 @@
         <v>40</v>
       </c>
       <c r="B42" s="2" t="n">
-        <v>208956</v>
+        <v>404435</v>
       </c>
       <c r="C42" s="2" t="n">
-        <v>4219</v>
+        <v>-5377</v>
       </c>
       <c r="D42" s="2" t="n">
-        <v>501.27</v>
+        <v>-775</v>
       </c>
       <c r="E42" s="2" t="n">
-        <v>0.34</v>
+        <v>-0.53</v>
       </c>
       <c r="F42" s="2" t="n">
-        <v>20.86</v>
+        <v>3.06</v>
       </c>
     </row>
     <row r="43">
@@ -9823,19 +9823,19 @@
         <v>41</v>
       </c>
       <c r="B43" s="2" t="n">
-        <v>204819</v>
+        <v>410344</v>
       </c>
       <c r="C43" s="2" t="n">
-        <v>4137</v>
+        <v>-5909</v>
       </c>
       <c r="D43" s="2" t="n">
-        <v>491.48</v>
+        <v>-844.64</v>
       </c>
       <c r="E43" s="2" t="n">
-        <v>0.33</v>
+        <v>-0.58</v>
       </c>
       <c r="F43" s="2" t="n">
-        <v>21.19</v>
+        <v>2.48</v>
       </c>
     </row>
     <row r="44">
@@ -9843,19 +9843,19 @@
         <v>42</v>
       </c>
       <c r="B44" s="2" t="n">
-        <v>200764</v>
+        <v>416810</v>
       </c>
       <c r="C44" s="2" t="n">
-        <v>4055</v>
+        <v>-6466</v>
       </c>
       <c r="D44" s="2" t="n">
-        <v>481.76</v>
+        <v>-917.53</v>
       </c>
       <c r="E44" s="2" t="n">
-        <v>0.33</v>
+        <v>-0.63</v>
       </c>
       <c r="F44" s="2" t="n">
-        <v>21.52</v>
+        <v>1.85</v>
       </c>
     </row>
     <row r="45">
@@ -9863,19 +9863,19 @@
         <v>43</v>
       </c>
       <c r="B45" s="2" t="n">
-        <v>196788</v>
+        <v>423854</v>
       </c>
       <c r="C45" s="2" t="n">
-        <v>3976</v>
+        <v>-7044</v>
       </c>
       <c r="D45" s="2" t="n">
-        <v>472.39</v>
+        <v>-993.27</v>
       </c>
       <c r="E45" s="2" t="n">
-        <v>0.32</v>
+        <v>-0.69</v>
       </c>
       <c r="F45" s="2" t="n">
-        <v>21.84</v>
+        <v>1.16</v>
       </c>
     </row>
     <row r="46">
@@ -9883,19 +9883,19 @@
         <v>44</v>
       </c>
       <c r="B46" s="2" t="n">
-        <v>192892</v>
+        <v>431502</v>
       </c>
       <c r="C46" s="2" t="n">
-        <v>3896</v>
+        <v>-7648</v>
       </c>
       <c r="D46" s="2" t="n">
-        <v>462.87</v>
+        <v>-1072.49</v>
       </c>
       <c r="E46" s="2" t="n">
-        <v>0.32</v>
+        <v>-0.73</v>
       </c>
       <c r="F46" s="2" t="n">
-        <v>22.16</v>
+        <v>0.429999999999998</v>
       </c>
     </row>
     <row r="47">
@@ -9903,19 +9903,19 @@
         <v>45</v>
       </c>
       <c r="B47" s="2" t="n">
-        <v>189073</v>
+        <v>439782</v>
       </c>
       <c r="C47" s="2" t="n">
-        <v>3819</v>
+        <v>-8280</v>
       </c>
       <c r="D47" s="2" t="n">
-        <v>453.74</v>
+        <v>-1155.43</v>
       </c>
       <c r="E47" s="2" t="n">
-        <v>0.31</v>
+        <v>-0.8</v>
       </c>
       <c r="F47" s="2" t="n">
-        <v>22.47</v>
+        <v>-0.369999999999999</v>
       </c>
     </row>
     <row r="48">
@@ -9923,19 +9923,19 @@
         <v>46</v>
       </c>
       <c r="B48" s="2" t="n">
-        <v>185330</v>
+        <v>448719</v>
       </c>
       <c r="C48" s="2" t="n">
-        <v>3743</v>
+        <v>-8937</v>
       </c>
       <c r="D48" s="2" t="n">
-        <v>444.7</v>
+        <v>-1241.74</v>
       </c>
       <c r="E48" s="2" t="n">
-        <v>0.31</v>
+        <v>-0.85</v>
       </c>
       <c r="F48" s="2" t="n">
-        <v>22.78</v>
+        <v>-1.22</v>
       </c>
     </row>
     <row r="49">
@@ -9943,19 +9943,19 @@
         <v>47</v>
       </c>
       <c r="B49" s="2" t="n">
-        <v>181661</v>
+        <v>458342</v>
       </c>
       <c r="C49" s="2" t="n">
-        <v>3669</v>
+        <v>-9623</v>
       </c>
       <c r="D49" s="2" t="n">
-        <v>435.91</v>
+        <v>-1331.93</v>
       </c>
       <c r="E49" s="2" t="n">
-        <v>0.31</v>
+        <v>-0.91</v>
       </c>
       <c r="F49" s="2" t="n">
-        <v>23.09</v>
+        <v>-2.13</v>
       </c>
     </row>
     <row r="50">
@@ -9963,19 +9963,19 @@
         <v>48</v>
       </c>
       <c r="B50" s="2" t="n">
-        <v>178062</v>
+        <v>468683</v>
       </c>
       <c r="C50" s="2" t="n">
-        <v>3599</v>
+        <v>-10341</v>
       </c>
       <c r="D50" s="2" t="n">
-        <v>427.58</v>
+        <v>-1426.44</v>
       </c>
       <c r="E50" s="2" t="n">
-        <v>0.3</v>
+        <v>-0.98</v>
       </c>
       <c r="F50" s="2" t="n">
-        <v>23.39</v>
+        <v>-3.11</v>
       </c>
     </row>
     <row r="51">
@@ -9983,19 +9983,19 @@
         <v>49</v>
       </c>
       <c r="B51" s="2" t="n">
-        <v>174538</v>
+        <v>479775</v>
       </c>
       <c r="C51" s="2" t="n">
-        <v>3524</v>
+        <v>-11092</v>
       </c>
       <c r="D51" s="2" t="n">
-        <v>418.67</v>
+        <v>-1525.26</v>
       </c>
       <c r="E51" s="2" t="n">
-        <v>0.29</v>
+        <v>-1.05</v>
       </c>
       <c r="F51" s="2" t="n">
-        <v>23.68</v>
+        <v>-4.16</v>
       </c>
     </row>
     <row r="52">
@@ -10003,19 +10003,19 @@
         <v>50</v>
       </c>
       <c r="B52" s="2" t="n">
-        <v>171082</v>
+        <v>491650</v>
       </c>
       <c r="C52" s="2" t="n">
-        <v>3456</v>
+        <v>-11875</v>
       </c>
       <c r="D52" s="2" t="n">
-        <v>410.62</v>
+        <v>-1628.4</v>
       </c>
       <c r="E52" s="2" t="n">
-        <v>0.28</v>
+        <v>-1.13</v>
       </c>
       <c r="F52" s="2" t="n">
-        <v>23.96</v>
+        <v>-5.29</v>
       </c>
     </row>
     <row r="53">
@@ -10023,19 +10023,19 @@
         <v>51</v>
       </c>
       <c r="B53" s="2" t="n">
-        <v>167694</v>
+        <v>504346</v>
       </c>
       <c r="C53" s="2" t="n">
-        <v>3388</v>
+        <v>-12696</v>
       </c>
       <c r="D53" s="2" t="n">
-        <v>402.5</v>
+        <v>-1736.68</v>
       </c>
       <c r="E53" s="2" t="n">
-        <v>0.28</v>
+        <v>-1.2</v>
       </c>
       <c r="F53" s="2" t="n">
-        <v>24.24</v>
+        <v>-6.49</v>
       </c>
     </row>
     <row r="54">
@@ -10043,19 +10043,19 @@
         <v>52</v>
       </c>
       <c r="B54" s="2" t="n">
-        <v>164373</v>
+        <v>517899</v>
       </c>
       <c r="C54" s="2" t="n">
-        <v>3321</v>
+        <v>-13553</v>
       </c>
       <c r="D54" s="2" t="n">
-        <v>394.58</v>
+        <v>-1849.67</v>
       </c>
       <c r="E54" s="2" t="n">
-        <v>0.28</v>
+        <v>-1.27</v>
       </c>
       <c r="F54" s="2" t="n">
-        <v>24.52</v>
+        <v>-7.76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>